<commit_message>
ajout graphiques de l'onglet statistiques
</commit_message>
<xml_diff>
--- a/admin_interface/initData/animals.xlsx
+++ b/admin_interface/initData/animals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perre\eclipse-workspace\Django\les_grandes_oreilles\admin_interface\initData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280930CE-3678-4D22-92B3-5271DDD24E79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCD6DBF-7C5C-439A-AA49-62A82C2E2360}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1548EE18-EDE2-4A6C-99F5-E0A8C3AE328A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
   <si>
     <t>id</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>2019-06-10</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -185,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -266,11 +269,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -287,6 +299,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA21FE66-6760-4D97-A962-08E5EF55779A}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -617,7 +632,7 @@
     <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -660,11 +675,12 @@
       <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="10" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
@@ -699,10 +715,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
@@ -735,10 +749,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
@@ -769,10 +781,8 @@
       </c>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
@@ -803,10 +813,8 @@
       </c>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
@@ -835,10 +843,8 @@
       </c>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
@@ -867,10 +873,8 @@
       </c>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
@@ -905,10 +909,8 @@
       </c>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
@@ -943,10 +945,8 @@
       </c>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Mise à jour de l'initdata en vue de l'integration des données
</commit_message>
<xml_diff>
--- a/admin_interface/initData/animals.xlsx
+++ b/admin_interface/initData/animals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perre\eclipse-workspace\Django\les_grandes_oreilles\admin_interface\initData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCD6DBF-7C5C-439A-AA49-62A82C2E2360}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4621AF48-288D-4B22-994B-6B8B06FE7198}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1548EE18-EDE2-4A6C-99F5-E0A8C3AE328A}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1548EE18-EDE2-4A6C-99F5-E0A8C3AE328A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
   <si>
     <t>id</t>
   </si>
@@ -95,30 +95,12 @@
     <t>Elsy</t>
   </si>
   <si>
-    <t>Nutella</t>
-  </si>
-  <si>
-    <t>Defy</t>
-  </si>
-  <si>
-    <t>Fran</t>
-  </si>
-  <si>
     <t>LAPIN</t>
   </si>
   <si>
     <t>PENSION</t>
   </si>
   <si>
-    <t>REFUGE</t>
-  </si>
-  <si>
-    <t>ABANDON</t>
-  </si>
-  <si>
-    <t>FOURRIERE</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -146,13 +128,52 @@
     <t>2020-03-10</t>
   </si>
   <si>
-    <t>2020-04-10</t>
-  </si>
-  <si>
     <t>2019-06-10</t>
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>perreautbis.clementine</t>
+  </si>
+  <si>
+    <t>callo.laurie</t>
+  </si>
+  <si>
+    <t>chaplin.charles</t>
+  </si>
+  <si>
+    <t>machado.chloe</t>
+  </si>
+  <si>
+    <t>gauger.sabine</t>
+  </si>
+  <si>
+    <t>serie.dexter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>2019-05-10</t>
+  </si>
+  <si>
+    <t>2020-02-10</t>
+  </si>
+  <si>
+    <t>2020-02-17</t>
+  </si>
+  <si>
+    <t>montant</t>
+  </si>
+  <si>
+    <t>date_sterilisation</t>
+  </si>
+  <si>
+    <t>poids</t>
+  </si>
+  <si>
+    <t>sante</t>
   </si>
 </sst>
 </file>
@@ -282,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -294,12 +315,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -616,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA21FE66-6760-4D97-A962-08E5EF55779A}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -632,7 +654,7 @@
     <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -675,311 +697,259 @@
       <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="10" t="s">
-        <v>39</v>
+      <c r="O1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="C2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" s="2">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>33</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2">
+        <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="1">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3">
+        <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
       <c r="F4" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="M4" s="1">
-        <v>22</v>
-      </c>
-      <c r="N4" s="1"/>
+      <c r="M4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4">
+        <v>100</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="C5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="8"/>
+      <c r="M5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="9"/>
-      <c r="M5" s="1">
-        <v>21</v>
-      </c>
-      <c r="N5" s="1"/>
+      <c r="P5">
+        <v>70</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="1">
-        <v>20</v>
-      </c>
-      <c r="N6" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="L6" s="8"/>
+      <c r="M6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="P6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="9"/>
-      <c r="M7" s="1">
-        <v>23</v>
-      </c>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="M8" s="1">
-        <v>21</v>
-      </c>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="M9" s="1">
-        <v>22</v>
-      </c>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="1">
-        <v>21</v>
-      </c>
-      <c r="N10" s="1"/>
+      <c r="L7" s="8"/>
+      <c r="M7" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="P7">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Corrections + ajout de nouveaux tarifs en parallèle des anciens
</commit_message>
<xml_diff>
--- a/admin_interface/initData/animals.xlsx
+++ b/admin_interface/initData/animals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perre\eclipse-workspace\Django\les_grandes_oreilles\admin_interface\initData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4621AF48-288D-4B22-994B-6B8B06FE7198}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499537D5-B3F0-463F-86B3-67341124AC21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1548EE18-EDE2-4A6C-99F5-E0A8C3AE328A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1548EE18-EDE2-4A6C-99F5-E0A8C3AE328A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
   <si>
     <t>id</t>
   </si>
@@ -71,9 +71,6 @@
     <t>date_dernier_vaccin</t>
   </si>
   <si>
-    <t>proprietaire</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -134,24 +131,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>perreautbis.clementine</t>
-  </si>
-  <si>
-    <t>callo.laurie</t>
-  </si>
-  <si>
-    <t>chaplin.charles</t>
-  </si>
-  <si>
-    <t>machado.chloe</t>
-  </si>
-  <si>
-    <t>gauger.sabine</t>
-  </si>
-  <si>
-    <t>serie.dexter</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -174,6 +153,108 @@
   </si>
   <si>
     <t>sante</t>
+  </si>
+  <si>
+    <t>Champ technique, ne pas remplir</t>
+  </si>
+  <si>
+    <t>Nom du lapin (tu peux mettre en rouge les doublons pour que je vois comment je les traite?)</t>
+  </si>
+  <si>
+    <t>Date de naissance si connue au format AAAA-MM-JJ</t>
+  </si>
+  <si>
+    <t>Date de première arrivée au refuge/à la pension si connue au format AAAA-MM-JJ</t>
+  </si>
+  <si>
+    <t>Date de prochaine visite veto si connue au format AAAA-MM-JJ (a priori pas de raison que tu la remplisse celle là)</t>
+  </si>
+  <si>
+    <t>Type d'animal. Valeurs possibles (respecter les majuscules): LAPIN, CHINCHILLA, COCHON_DINDE</t>
+  </si>
+  <si>
+    <t>Emplacement actuel de l'animal, valeurs possibles : PENSION ou REFUGE</t>
+  </si>
+  <si>
+    <t>Origine de l'nimal s'il est entré au refuge. Valeurs possibles: ABANDON, REFUGE, FOURRIERE, AUTRE</t>
+  </si>
+  <si>
+    <t>Sexe : M ou F</t>
+  </si>
+  <si>
+    <t>Stérilisé : OUI ou NON</t>
+  </si>
+  <si>
+    <t>Vacciné : OUI ou NON</t>
+  </si>
+  <si>
+    <t>Date de dernier vaccin si connu, au format AAAA-MM-JJ</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Prénom</t>
+  </si>
+  <si>
+    <t>Nom du propriétaire</t>
+  </si>
+  <si>
+    <t>Prénom du proprietaire</t>
+  </si>
+  <si>
+    <t>PerreautBis</t>
+  </si>
+  <si>
+    <t>Clémentine</t>
+  </si>
+  <si>
+    <t>Callo</t>
+  </si>
+  <si>
+    <t>Chaplin</t>
+  </si>
+  <si>
+    <t>Machado</t>
+  </si>
+  <si>
+    <t>Gauger</t>
+  </si>
+  <si>
+    <t>Serie</t>
+  </si>
+  <si>
+    <t>Laurie</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Chloe</t>
+  </si>
+  <si>
+    <t>Sabine</t>
+  </si>
+  <si>
+    <t>Dexter</t>
+  </si>
+  <si>
+    <t>Description général de l'animal</t>
+  </si>
+  <si>
+    <t>Date d'adoption pour les animaux adotés au refuge au format AAAA-MM-JJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montant de l'adoption pour les animaux adotés au refuge </t>
+  </si>
+  <si>
+    <t>Date de stérilisationsi connu, au format AAAA-MM-JJ</t>
+  </si>
+  <si>
+    <t>Poids si connu</t>
+  </si>
+  <si>
+    <t>Descriptif santé</t>
   </si>
 </sst>
 </file>
@@ -195,7 +276,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,8 +289,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -299,11 +386,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -324,6 +431,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,23 +764,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA21FE66-6760-4D97-A962-08E5EF55779A}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6328125" customWidth="1"/>
+    <col min="2" max="2" width="35.7265625" customWidth="1"/>
     <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.90625" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="23.36328125" customWidth="1"/>
+    <col min="7" max="7" width="17.08984375" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" customWidth="1"/>
     <col min="12" max="12" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.90625" customWidth="1"/>
+    <col min="14" max="14" width="24.26953125" customWidth="1"/>
+    <col min="15" max="15" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -692,262 +824,341 @@
         <v>11</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="117" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="S1" s="11" t="s">
-        <v>46</v>
+      <c r="C3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3">
+        <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="P3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4">
+        <v>30</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>29</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="8"/>
-      <c r="M5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="P5">
-        <v>70</v>
+      <c r="M5" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" t="s">
+        <v>64</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5">
+        <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>25</v>
+      <c r="K6" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="L6" s="8"/>
-      <c r="M6" t="s">
-        <v>37</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="P6">
-        <v>10</v>
+      <c r="M6" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" t="s">
+        <v>65</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6">
+        <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="L7" s="8"/>
-      <c r="M7" t="s">
-        <v>38</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="P7">
+      <c r="M7" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" t="s">
+        <v>66</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="8"/>
+      <c r="M8" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" t="s">
+        <v>67</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q8">
         <v>80</v>
       </c>
     </row>

</xml_diff>